<commit_message>
#24 gulftalent result is now filtered based on loc coming in api requets
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,66 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Freelance Project\job-scraper-backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724B61C8-3CE8-4069-B6A2-3E239A91151E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>JobTitle</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>PostDate</t>
-  </si>
-  <si>
-    <t>JobUrl</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,32 +48,91 @@
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Heading" xfId="1"/>
+    <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Result" xfId="3"/>
+    <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -389,33 +420,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>JobTitle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>PostDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>JobUrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Programmer</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>RTC-1 Employment Services</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dubai, UAE</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>97 days ago</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.gulftalent.com/uae/jobs/programmer-316493</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Programmer</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>RTC-1 Employment Services</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Dubai, UAE</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>41 days ago</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.gulftalent.com/uae/jobs/programmer-320201</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Programmer/Developer</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Convilguous DWC-LLC</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dubai, UAE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>136 days ago</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.gulftalent.com/uae/jobs/programmer-developer-314427</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Linkedin scrapping rules and login with the help of selenium
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20376" yWindow="-120" windowWidth="20736" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -425,100 +425,344 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>JobTitle</t>
+          <t>Kotlin Developer – Full-time, Remote</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Company</t>
+          <t>Toptal</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>PostDate</t>
+          <t>Dubai, Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>JobUrl</t>
+          <t>https://www.linkedin.com/jobs/view/2648921423/?eBP=CwEAAAF6sFnSRCwq5yeVOz3lshQnKtwaXvffo3zRe0WIOMsL3YG-ZpZVIBMvLn9_9Gg9TCdDSdJZV0Hyw5FDjEMzMI5cz_FoWfwBkpuYjqAMaMSx3WQ6WkNg_dIky8ujmtX1wq7erWFq7TZcwDzQ3f6I4Xth_TqroVAQjD9seATVb1vo_xrPRjW9FPlzcfIYud-fUKvefkNkxN7DU_EowIKOo2LHfHedDFiMNeMfGwDQCBDPmA_6tDkp1__vfz1TgC2m-zE8hLBezIUMGVB5rzLWyc1fQ20UomzN7a_vfR0kYSzxF2zymghJYoCK2qf5kxMfru64SMbS7kubsyu_-OzkVzpysCRSGFbxAbYUQoSV_EivSouNmAFnljvdG83H&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=IQ08OXcRjo1ksy7zwvcxwA%3D%3D&amp;trackingId=qmfYMMQ33yhTaibFpRih7g%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>Senior C++ Developer – Full-time, Remote</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Arab Payment Services (APS)</t>
+          <t>Toptal</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dubai, UAE</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>64 days ago</t>
+          <t>Dubai, Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.gulftalent.com/uae/jobs/backend-developer-317833</t>
+          <t>https://www.linkedin.com/jobs/view/2637116275/?eBP=CwEAAAF6sFnSRY3SupZg-UcGKeEKvkm77turW9ynZpV6gFC99HQkVQiCICnjCEFctuG0wopCyPPIRbdSJhvFdPUsbe3vXZbhRRbs92iChk4pMN1A6SHDFDRCpT46Ivzdtpu-G7Aa4PbC9moCmZs3N1AXSEkBL50ZcHrl5cjdzyMKiNIfqVWUiPya-2GaPmT3xvn6AOzknisDIwt4TN3UZTXIutPXsn_qfv2n28LVYKyZsOYh3JwQm5j-bk_KZAtVMr08zdrZKF0dkemg8vxet2utIjZn4k9MLJj8zuBpB_IgiV6RvnkBsvcSAMzbwxUzrFMRr-eq7cFIVWvlw_XtegcaTbXAs2h-RWS8E9Qg-IqGV8n46xPXgS9JBLBdfFyk&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=IQ08OXcRjo1ksy7zwvcxwA%3D%3D&amp;trackingId=eRMZ5rfytaY3q5a4bfIUGQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>Senior Software Engineer - iOS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Arab Payment Services (APS)</t>
+          <t>HungerStation | هنقرستيشن</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dubai, UAE</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>64 days ago</t>
+          <t>Dubai, Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.gulftalent.com/uae/jobs/full-stack-developer-317835</t>
-        </is>
-      </c>
+          <t>https://www.linkedin.com/jobs/view/2631668884/?eBP=CwEAAAF6sFnSRX4kM6Cb5n08ZX2qvHjeLgslll6OaPb5lD2xPJ9WjXUokMr6NSrfqO0vY2UTaffT1ii9SBAPXd25l5hS7XX7U0UVgiD2IX4PwUk_mUwNWAcY3GyIpBAkFS79XtjZls8ASZc0EEZsc4QKDocpWcv7JqNAwkOXg52ma1wQIDmpbYJdy66tvHv1urrhrix68GBg9787tVHuO7KCLYd2Chy4H93k8Rs5eGk5ug0Sf_FbzxBNwdQabZdUfnf5_1mr0N2ep0Lc4NWd5GIHZwyvSaUPt-MqTyk7Wx9a4HVN2bP80xnQseuop-mDyMS_FNG7MCzT8FkTmPYVshyZyIvghEcIZjVoyCvCMtO3D0ia5fVXxrvjODT4ur3Q&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=IQ08OXcRjo1ksy7zwvcxwA%3D%3D&amp;trackingId=huPKmoZECG9Euxzb2aJ8zQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MuleSoft Developer (On-site)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Halian</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+              2 days ago
+ </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2643770873/?eBP=JOB_SEARCH_ORGANIC&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=IQ08OXcRjo1ksy7zwvcxwA%3D%3D&amp;trackingId=petFiK%2BrK7UyfAmDkzxoFQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer I - Android</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>talabat</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Business Bay, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2636396773/?eBP=CwEAAAF6sFnSRYP6wJETgDUt_BTRuRrvqb3UmnGfNJR10NZ5crRzyjrz53oHiu-VI9EfEilJ6BYTvbDgRL0iXWb0PJDn9gByXcRErBIOQyHfGWbTaahvz8hhYpCIoPARe6tqm9Xxl6Nm2JQ7YGiA_La1ZBxuGzCUdAZRBWjGK8X23N7Dyw9PQjGUc5XpJfhNXBE2NhB6JNEORIawBArmxrjAZKh3dBfgto7wM4HGNMQgd2O4_UYxdhh-qd83AmTAh6j9o4iefJIaFxexDF9B4sklfLjhjUYUE1Ze4w1xAdngzdAh4pvcrj7MzKpYCrX6Az0mYx3qt7vcJU4wT72iDGQnfAEeErvtiuQTubBJvp-5RDGqE5RVVFERZUj-og&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=IQ08OXcRjo1ksy7zwvcxwA%3D%3D&amp;trackingId=XSF1GYCf6L3CCXgvzuHgqA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Analyst Programmer</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Element Materials Technology</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2596932004/?eBP=CwEAAAF6sFnSRYphO-XBYBC_9I24OFOQwsoWvvtZHkfsCkcZ4zgx6xvmyFJhRJXWRBb4BrWayHpzWZD8fk9Bk6RtaGsueDDAu7Xl9fRY8H8FkDK7lLt3QpSlbd3BVlNMpzQHzpSfpCnSE255WMf6qIFHegkQju1dR7N2_HfA6-uPnrD4d3lgPgwpZAN9Y2RIV9MFpUdLORt0nVcYVfmzNvla7Rf4xrNoevE8Jc9mBYjCoLJzwHWsIUFjm0SQhl47hf60rgALmhdYAXeNRUIQ1ZR-DelSejNWOtg4RCFqXh405HNGYUJDO5osib6XI-D0qpdwzI_iHuYYMWCqJnccznX3fKSbFAdTd7ASPhf8nOc94mT_GQVx4IlD7ANgvKD633c&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=IQ08OXcRjo1ksy7zwvcxwA%3D%3D&amp;trackingId=8EIaaLeSqWGMp8w%2FFKfzrw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - Backend</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>HungerStation | هنقرستيشن</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2632660011/?eBP=CwEAAAF6sFnSRTVNVugTMdlPYgBqFZ4uxLfuC5wunFkmCfr-yeWCoBqrc3CRSPtrdD6iTqVXAjQ_5HOnbKGoqRBStqCr7cF-2DrqOF1G41q6cWrcwOPksSeNIIkFBxRvQc4qCPHANqWzFXVjArSkCqbW-ZraQbnGQd68nEnbMBd0gfleUX_ERrAiN3NxvA8LGlgsJmX4iBKypn8D_0biYrLvavlfUM6IuMVjVsWs16Vb0p2vI59U1dkQGb8Dk1EYpF-vofuVF_b-3--PYqoMFmjIFZJoiZBjVAC6QqnyzIo47rBP58F_XBIjfojcodv6ccnnFu9PoLcLe9M1c5EyY2B7khHb4ihoNIPyyk4hD035R1Pksdr0n3dQMIC4NQ&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=IQ08OXcRjo1ksy7zwvcxwA%3D%3D&amp;trackingId=maVlzUTwp%2F5D1nwlOM%2BvbQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Kotlin Developer – Full-time, Remote</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Toptal</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2648921423/?eBP=CwEAAAF6sGCRLNffWS3pcIqKajJonH2AaqFyPzJ4TpLMPT5BYqsILnNN47bGAFhDP6KQkuKyQLjgIVjWGN5nMIFKIk911wh2yOWNkZrb6aSN0bFLm75DS_DUzj7FoAa8OtVTVqJ1W1rSvsFnwGLZJtwCS9SthGwCneSlpwkuHBjD7DgYNeSx-RRoQ7TD8_YZQvog1wrjTqyywTIhuN0P3feo6RtNmU-KEkkiJLx78CsP9GPgh1CqOQYSea0cqv8NcAfaySzSc1vNT3Vl-j0mdAg8O_ze9Acl408KT9iRASHIZL9RbxJF8t3bzJ4Bu6XYQ98l8W6aLI-kRxLzi3l_Zl6PmtBYJi_0M9fO6v1lEARrOoznZZI9oRyXEH--Yh1Th4pAnQ&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=GZ2xbL4fakYgxg1w%2FA5t%2FA%3D%3D&amp;trackingId=9wVIa3Cfw%2Fm9r4IFU7x4Pg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Senior C++ Developer – Full-time, Remote</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Toptal</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2637116275/?eBP=CwEAAAF6sGCRLL0gJcxrUp35wUAclZE6LQAeeUXI7irc05gI2ae7TCDW27l5G77cq92QpTIH0S2rqITGilVUgDdXhT8Vp38OSVtcGJGgiVAVL-0NdglDIskOjyqNXJzdjuwiSUiOBAaCNNrn5wog0Z1hwBQgNGZ3VlJhmmKU75DB6kOT6LoBSfml9RrHAxowBmduAPL_Jggr_rlwCBvFTg3V2LgTAB3hbyu6UjfEljBoW8N9q18FNbTS497CFcv1vyUO4S_0k0Qx4yx72AooU08Z3yAXCNLeszZU-SJiRTY8Dh15cPVp7xoADJsHv_YbSNTlfO68uq12pe8xhSQg5D5HnGKA85eNXhEKERx_O4n3uHVlXV8BnrzAFP0MzKN5N66yeg&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=GZ2xbL4fakYgxg1w%2FA5t%2FA%3D%3D&amp;trackingId=KB2WDJ8XJHOGAFjH8sHjJg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - iOS</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>HungerStation | هنقرستيشن</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2631668884/?eBP=CwEAAAF6sGCRLItbkls_7TwLGQ6rsgz4PyunNjv5HGQNN-e7dOaCzWfAC4mUx-ZVpndgELD_ujCkaYSSwUKSNNqmcavVZjdGIVM99gaaCpw4SdSLRmq30YthZbe3pIYO8O2KaIsfkbQO6BfUmkHpM_1zZ1v0JeQ-FydYBizn6qXJVXY8QX1d_-JBah_S85TSHRxfeEdwxwbm9eWkvfwxF21lVogbw-Zhvjj8DT0cNX0_v_j1bTk-fI2gmdI2PxQgSGFFpjwwQJXKTKYsdRrFgLuwtDUCQTxrYR8vHIWZypaYhgk90gavBmEWGSZI3rTC17CHTAI1VPjNRJR9linC7PJPtoi_lC_XT18x7vUovB2ULZ7_wS4tKRWvZxsRL1M1YlU&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=GZ2xbL4fakYgxg1w%2FA5t%2FA%3D%3D&amp;trackingId=IIwtSF%2BEskNLZGcx%2BdEL%2FA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>MuleSoft Developer (On-site)</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Halian</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+              2 days ago
+ </t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2643770873/?eBP=JOB_SEARCH_ORGANIC&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=GZ2xbL4fakYgxg1w%2FA5t%2FA%3D%3D&amp;trackingId=xT3lv4vxWVcffR7nvrvHUQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer I - Android</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>talabat</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Business Bay, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2636396773/?eBP=CwEAAAF6sGCRLFstEgneMknLFNynKuv4n2hq7Vf2FLrvwj4d4TXId0bSRyJIXaIn46GxH6Vl5cgHPk87KVrASGkOtx6E5MbldWhDGa01CJn7ev8UIj7KdB-DO3Ve_BOyNDWAmo_hmhjIG9sFZTF0uu2JWzcRSMLi2eAcPikSRapC4mVZwwcO01flEmda3hCTXSJPCotZNVYTiQi8wldIonMonQVbBPSevgwMoT2zpAKA_K_OTyF_PJ4T0t_DbiuwFS74icvDHHxYTFHFevjKAULsdniAsxHekuv3KCa2gLaVVk2KjSAdFhq60tWMHKqTwkujpz1Id_GnHITLHBdoVUXETgTsjVO-w7xg6UKOgzjdSDyAI_N1FQMhGrjT1lh2JYtC-w&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=GZ2xbL4fakYgxg1w%2FA5t%2FA%3D%3D&amp;trackingId=b7b0Yd0sShh6bogMbXCfGQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer - Backend</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>HungerStation | هنقرستيشن</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2632660011/?eBP=CwEAAAF6sGCRLA0oWWdl2n4MX2NIapZz6HvKN7x_RkwRoYRndueWy7Fpi-HCfE2nZJDG4ed1JnMttGAaC5A7raLdhcXzyuQ550m6de2CQSrZOIMpGalrSqvWAXBifBxQoPQEcdZR38TsPnJ57hhDBnvWDWELnci6toYX78Afh3CbhFx1ufc04VYh_wojACHR8luKraRkGjaxGHgC_WctNfPIqyneW2xH4-mGSR2tIx96G2f-cCGHkcj64wzggHXwdwTz-shYCfOEPSHEihXU3-yLlNvl8NQZM6DlsxOg1Eh52dTWQgWUU-LCWCh9RNwBqAaoo-GzWJXHH9rMHApr9TT2zM03J_xFrvnLg_Z-aM6dZ2vILD3TuygIjZ1FeCQbOHAySQ&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=GZ2xbL4fakYgxg1w%2FA5t%2FA%3D%3D&amp;trackingId=oxbwDZMI9epbV0gicXUa%2Bg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Analyst Programmer</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Element Materials Technology</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Dubai, Dubai, United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/2596932004/?eBP=CwEAAAF6sGCRLHmy1_cE9GM9WsDXd5AFzaMuuiLawfDlvN21zzvRRfgZWwDGOnCGSnmj8M2zakmcUqO9Qbex5WyU84XAnptTKwJERgFUKjnHlFRAFMQjxC6t3qshN3XhYhXh1vKJKhCn2aTYqn0BTyUodItcUhjKe4yVD5XQqJJ8uuwoKFisO9jb5sjc2dditp1y5sBDzWrUlrWYs9MqlUHOEKcd2C9wyal1g6rb2U9yxPxNL0RNyMIqWC1yAjPpvxU1g9HlQsWpPzCo1ikD4bKJ3pHSTtJQFrbe9hXAjedj-ED8wYLi-mmRGTY1aKBV9pEbz1UJGEY0Sv5Xgsq-huMm656_O7_8BIBww16J9oXSyAh5wNH-d3S7p7gpfgTNjpyPOOfB&amp;recommendedFlavor=ACTIVELY_HIRING_COMPANY&amp;refId=GZ2xbL4fakYgxg1w%2FA5t%2FA%3D%3D&amp;trackingId=YN3cKGE2ZZjFeMSzAdIhKA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="49"/>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed indeed posted data error
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,495 +468,960 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Manager in Training (MIT) Program - Middle East</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Louis Vuitton</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>As part of Louis Vuitton’s Manager in Training (MIT) Program, you will embark upon a dynamic and in-depth journey of discovery through 4 phases: Client advisor…</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Posted4 days ago</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-at-3db-events-2672870467?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=z%2FdQXLtwy9Ww%2BN9L6bEEiQ%3D%3D&amp;position=2&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=7141066c9fc08d8a&amp;fccid=1807e5727f702882&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Senior Project Manager</t>
+          <t>General Manager - Luxury Resort</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Michael Page AE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t> At least 10 years of experience in the executive management of operations, sales and marketing, food and beverage or related professional area of luxury…</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>7 days ago</t>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-at-mashreq-bank-2661664425?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Vie%2FuJLL%2FOTybROPRC9Pqg%3D%3D&amp;position=3&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=f15a7ddaf4d3bef8&amp;fccid=77087bd1709a8148&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Assistant Department Manager LG</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Christian Dior Couture</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Follow up with the Department managers to ensure optimization of the stock level usage.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Posted25 days ago</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-at-sana-commerce-2672381177?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=ad9YZ53J04vbiwH5%2BUPXBA%3D%3D&amp;position=4&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=5b0e5213019a6fd8&amp;fccid=6a2be34af774e2bb&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Duty Manager</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Anantara</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Abu Dhabi</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Should be a strong and experienced hotel ambassador who excels at maximizing the experience and satisfaction of the hotel guests.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3 days ago</t>
+          <t>Posted16 days ago</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-at-talents-uae-2669842845?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Zdn5QfCkeRBY6CCIqD86RA%3D%3D&amp;position=5&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=850fad99487d4240&amp;fccid=2af5b593acca1f1f&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Assistant Manager - Dubai Mall</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tiffany &amp; Co</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>A minimum three year’s retail leadership experience within a luxury retail environment.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-at-relience-ltd-2660025196?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Mor8Owtv7tz7n2205JU0vw%3D%3D&amp;position=6&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=bfca47ad77a2ebea&amp;fccid=329e52936d287237&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Senior Project Manager</t>
+          <t>Regional Retail Manager - Premium Luxury Brands</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Working as a Retail Manager you will be responsible for ensuring that Store Directors/Managers maximise the commercial performance of their retail shops and…</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-at-turner-townsend-2667149378?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=nUSNuvGOhNG6uOdlY8DHig%3D%3D&amp;position=7&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=3d46626a0e65ba12&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Freelance Project Manager</t>
+          <t>Boutique Manager - Al Ain Mall</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Chanel</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Abu Dhabi</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>You have at least 5 years’ experience in boutique management in a luxury retail environment preferably in fragrance and beauty.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2 days ago</t>
+          <t>Posted12 days ago</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/freelance-project-manager-at-prolab-digital-llc-2667910346?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Y%2Bhph4lhnfpCyrwCEkAkAQ%3D%3D&amp;position=8&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=15c6e1d5546301f2&amp;fccid=20f48cf7726b0510&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Showroom Manager – Africa</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Danube Group</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>This luxury furniture is made with the highest quality, all-natural, material.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>Posted13 days ago</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-at-sign-works-llc-2655714103?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=JuAtESQa7WwLycNHTTkHzw%3D%3D&amp;position=9&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=f24791aa7942acd7&amp;fccid=a6bec4b75595280e&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Retail Design Project Manager</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>L'Oreal</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Remote in Dubai</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Within the Retail design and visual merchandising department, the Retail design project manager will be in charge of the implementation of the permanent POS …</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4 weeks ago</t>
+          <t>Posted9 days ago</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-at-elsewedy-electric-2640119108?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=vViY37keANgTLM537puG%2Bg%3D%3D&amp;position=10&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=1d7504e169401aed&amp;fccid=ec8a0bd60be9a6f5&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sr. Project Manager</t>
+          <t>Retail Manager - Guerlain</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>The Regional Retail Manager is responsible for sales objective achievement and outstanding omnichannel client experience across the retail network (boutiques…</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4 weeks ago</t>
+          <t>Posted3 days ago</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/sr-project-manager-at-epsilon-global-consulting-2629795302?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=tZ%2F%2BFxYntDPUtGcDMpV4Rg%3D%3D&amp;position=11&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=c183b9675d782014&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Project Manager - Fitout ( Talent Pool)</t>
+          <t>Market Development Manager - Dubai, UAE</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Argyll Scott MY</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Up to UAE Dirhams384000 per annum per annum.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>Posted5 days ago</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-fitout-talent-pool-at-al-tayer-group-2667969953?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=zBlXWKyUeegLp9aeUSgePw%3D%3D&amp;position=12&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=cc0a01bd82e90fc5&amp;fccid=91277dc7f9bcbc55&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Brand Project Manager</t>
+          <t>Senior Regional Manager - Luxury Fragrances - MEA Coverage</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Michael Page AE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Reporting to the Managing Director, this person will be responsible for;</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/brand-project-manager-at-noon-2644357673?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=ifezvT9WQ2zL%2B9ZRDnF%2Btw%3D%3D&amp;position=13&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=f14fd6c319542ff6&amp;fccid=77087bd1709a8148&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Project Manager - Pavilion (Expo)</t>
+          <t>Team Manager - Client Service Center</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Louis Vuitton</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Manage and motivate the team to drive business: create a positive and harmonious work environment, foster cooperation within the team and between managers.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Posted20 days ago</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-pavilion-expo-at-world-security-2668921191?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=rjKJp06bTArPYOeKUYGUAw%3D%3D&amp;position=14&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=add0a2677658044d&amp;fccid=1807e5727f702882&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Project Manager (Change &amp; Transformation) - 1 year contract</t>
+          <t>Night Manager</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Marriott International, Inc</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Assists operations manager in processing employee payroll weekly.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4 weeks ago</t>
+          <t>Posted13 days ago</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-change-transformation-1-year-contract-at-commercial-bank-international-2631901808?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=yutsJnY5Z%2BXKiLCdy4LYGw%3D%3D&amp;position=15&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=ffbdce9fa2d04545&amp;fccid=0b6c496064ecd79a&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Head of Project Management</t>
+          <t>Assistant EBC Manager</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Marriott International, Inc</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Contact appropriate individual or department (e.g., Sales, Data Administration, Accounting) as necessary to resolve guest calls, requests, or problems.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>Posted2 days ago</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/head-of-project-management-at-encore-2656362283?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=cROBuarnmkEXbQw2KbGcvg%3D%3D&amp;position=16&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=1b0e4e550137f8a7&amp;fccid=0b6c496064ecd79a&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Project Manager - 6 mths contract</t>
+          <t>MEA Logistics Manager</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Luxury Goods International (L.G.I) SA (Branch)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Based in Dubai, the MEA Logistics Manager supports the development of the Kering Brands’ business by implementing and running best-in-class logistics solutions…</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-6-mths-contract-at-manpowergroup-middle-east-2662326668?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=TLfuvvRxY%2B9jAullaA%2B%2B4g%3D%3D&amp;position=17&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=3de3673c2ca392d7&amp;fccid=dd616958bd9ddc12&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Senior Project Manager</t>
+          <t>Sales Delgate/ Junior Area Retail Supervisor</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SSC Perfumes &amp; Cosmetics</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>LVMH P&amp;C Middle East oversees an area of 47 countries in the Middle East, Europe, Africa, and India with subsidiaries and agents’ structures.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>Posted25 days ago</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-at-hantec-markets-2655474696?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=m1UsVaYW7r0%2BjyEXWiRWdw%3D%3D&amp;position=18&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=57d8e49629b99c35&amp;fccid=5ad360b814db19a5&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IT Manager - Projects / Events</t>
+          <t>Senior Project Manager - Store Renovation - Level Shoes</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Remote in Dubai</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Excellent time management with capabilities to multitask with a strong understanding of core manager duties.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3 days ago</t>
+          <t>Posted18 days ago</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/it-manager-projects-events-at-falcon-and-associates-2667213702?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Tu1UzYIXsjzh0aVjxSbpIg%3D%3D&amp;position=19&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=1e399b9031998ae9&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Innovation Project Manager</t>
+          <t>Clienteling Manager – CELINE Dubai Mall</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Support store managers in managing their teams on customer issues.</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Posted20 days ago</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/innovation-project-manager-at-dnata-2666301640?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=bgYKmmUumYFHJbS9Gi4dtw%3D%3D&amp;position=20&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=72cd01f90905f251&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Technical Project Manager (Location-Based)</t>
+          <t>Assistant Manager - Dubai Mall</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Tiffany &amp; Co.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>A minimum three year’s retail leadership experience within a luxury retail environment.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/technical-project-manager-location-based-at-magnopus-2655085650?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=7EN2M31T8kDc4Vu3WXV9RA%3D%3D&amp;position=21&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=83b998ce18b6cb88&amp;fccid=329e52936d287237&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Senior Project Manager - Hotels (FE-PM)</t>
+          <t>Private Client Manager</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FARFETCH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Through a variety of engagement and selling activities, you'll ensure a seamless, exceptional luxury shopping experience for our Private Client customers.</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/senior-project-manager-hotels-fe-pm-at-fifthedge-construction-recruitment-intelligence-2672670876?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=wMoWfNN0vSEq6hfYocyUEw%3D%3D&amp;position=22&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=b098d592cdae6db1&amp;fccid=9f5fb2f8ae2fcc49&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Project Manager - IT</t>
+          <t>Private Client Assistant Stylist</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FARFETCH</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>We're looking for someone with strong customer service skills and knowledge of the luxury fashion market who is driven to achieve targets.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1 month ago</t>
+          <t>Posted2 days ago</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-it-at-majid-al-futtaim-2658682541?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=Ex5Y3Uv91M2XETYWeTJEsw%3D%3D&amp;position=23&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=0123577ae0ac18b3&amp;fccid=9f5fb2f8ae2fcc49&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Senior Manager, New Solutions</t>
+          <t>Area Retail Manager – Luxury Brand</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Charterhouse Consultancy PTE Ltd</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>The main purpose of this role is to meet the business objectives, drive the performance and maximize the profitability of all the assigned stores, recruit,…</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/senior-manager-new-solutions-at-visa-2666391375?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=zQrHnnvWj4x8fR1dxVQ5tA%3D%3D&amp;position=24&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=058b3df0807cd28e&amp;fccid=4749f34298e2e970&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Project Manager</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
+          <t>E-Commerce Manager</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>coty</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Dubai, Dubai, United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>You will be responsible for developing and overseeing the brands online sales, seamless user experience and customer journey on the web.</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>6 days ago</t>
+          <t>Posted30+ days ago</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://ae.linkedin.com/jobs/view/project-manager-at-servion-global-solutions-2659556427?refId=cWmE%2B0M8h1r2qi3LmtQJtg%3D%3D&amp;trackingId=JibrnQFBhga8mRrgGoejyQ%3D%3D&amp;position=25&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+          <t>https://ae.indeed.com/rc/clk?jk=f2ede358b9f91676&amp;fccid=7ad46606e93080a6&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Quality Assurance Manager - Emirates Academy of Hospitality Management</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Jumeirah</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>The Quality Assurance Manager is directly responsible to the Dean, EAHM, for the accurate and effective reporting of institutional data, academic performance.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Posted30+ days ago</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=17a460bfdfebc7fd&amp;fccid=8015c178481add76&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Junior Area Retail Manager - Guerlain</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>As Junior Area Retail Manager, you will be responsible for supporting the Area Retail Manager within Guerlain for Travel Retail for the region.</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Posted20 days ago</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=8793ce2c66d0caff&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Recreation Manager</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Oversee the smooth running of the Sports &amp; Recreations department on a day to day basis to achieve the highest possible levels of guest satisfaction.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Posted27 days ago</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=41d202b8068a372c&amp;fccid=2af5b593acca1f1f&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Strategy Manager</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>The Strategy Office provides the organisation with an overall compass, based on the Group’s vision and directions previously defined.</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Posted30+ days ago</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=3794f02a2013b247&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Senior Visual Merchandiser - Luxury Fashion - Abu Dhabi</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Chalhoub Group</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Abu Dhabi</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Communicate with retail manager on impact of new merchandising on sales.</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Posted6 days ago</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=df472563e2b34dd6&amp;fccid=01f47b3f00b281a4&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Property Manager</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Asayel Investment</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Abu Dhabi</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Budgeting. • Real estate financial analysis.</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Posted30+ days ago</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://ae.indeed.com/rc/clk?jk=16b9779594f116f3&amp;fccid=f697fec203d7893a&amp;vjs=3</t>
         </is>
       </c>
     </row>

</xml_diff>